<commit_message>
Update Power Budget Example-1-1 (1).xlsx
</commit_message>
<xml_diff>
--- a/Docs/Power Budget Example-1-1 (1).xlsx
+++ b/Docs/Power Budget Example-1-1 (1).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofstthomasmn-my.sharepoint.com/personal/frie9722_stthomas_edu/Documents/Final_Project_ENGR331/dawg-security-system/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofstthomasmn-my.sharepoint.com/personal/frie9722_stthomas_edu/Documents/Final_Project_ENGR331/dawg-security-system/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{4611DB46-3A12-4BFB-933A-5CA77827C030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1308E00A-F600-4364-BA07-16E0D05A8841}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{4611DB46-3A12-4BFB-933A-5CA77827C030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB8D3C0D-86F4-4F9D-8607-7EA2B4457F1E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -201,9 +201,6 @@
     <t>Ultrasonic Sensor</t>
   </si>
   <si>
-    <t>Buzzer/Speaker</t>
-  </si>
-  <si>
     <t>LED (*4)</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t xml:space="preserve">Send Alerts </t>
+  </si>
+  <si>
+    <t>Buzzer/Speaker ()</t>
   </si>
 </sst>
 </file>
@@ -998,18 +998,72 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="37" xfId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1037,15 +1091,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1054,51 +1099,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1117,6 +1117,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1388,7 +1392,7 @@
   <dimension ref="A1:V25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1407,55 +1411,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F1" s="81" t="s">
+      <c r="F1" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
     </row>
     <row r="2" spans="1:22" s="1" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="82" t="s">
+      <c r="A2" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82" t="s">
+      <c r="G2" s="53"/>
+      <c r="H2" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82" t="s">
+      <c r="K2" s="56"/>
+      <c r="L2" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="85"/>
-      <c r="L2" s="82" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="82"/>
-      <c r="N2" s="63" t="s">
+      <c r="M2" s="53"/>
+      <c r="N2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64" t="s">
+      <c r="O2" s="82"/>
+      <c r="P2" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="56" t="s">
+      <c r="Q2" s="82"/>
+      <c r="R2" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="58"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+      <c r="U2" s="76"/>
       <c r="V2" s="34"/>
     </row>
     <row r="3" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1510,10 +1514,10 @@
       <c r="Q3" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="59"/>
-      <c r="S3" s="60"/>
-      <c r="T3" s="60"/>
-      <c r="U3" s="61"/>
+      <c r="R3" s="77"/>
+      <c r="S3" s="78"/>
+      <c r="T3" s="78"/>
+      <c r="U3" s="79"/>
       <c r="V3" s="9"/>
     </row>
     <row r="4" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1545,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="40">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="K4" s="41">
         <v>0</v>
@@ -1558,7 +1562,7 @@
       </c>
       <c r="N4" s="22">
         <f>(SUM(F4,H4,J4,L4))/3600</f>
-        <v>4.7222222222222221E-2</v>
+        <v>6.9444444444444448E-2</v>
       </c>
       <c r="O4" s="23">
         <f>(SUM(G4,I4,K4,M4))/3600</f>
@@ -1566,18 +1570,18 @@
       </c>
       <c r="P4" s="19">
         <f>(B4*N4)+(D4*O4)</f>
-        <v>0.60000000000000009</v>
+        <v>0.68888888888888888</v>
       </c>
       <c r="Q4" s="15">
         <f>(C4*N4)+(E4*O4)</f>
-        <v>0.86944444444444446</v>
-      </c>
-      <c r="R4" s="68" t="s">
+        <v>1.0472222222222223</v>
+      </c>
+      <c r="R4" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="69"/>
-      <c r="T4" s="69"/>
-      <c r="U4" s="70"/>
+      <c r="S4" s="84"/>
+      <c r="T4" s="84"/>
+      <c r="U4" s="85"/>
       <c r="V4" s="33"/>
     </row>
     <row r="5" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1606,7 +1610,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="44">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="J5" s="42">
         <v>0</v>
@@ -1626,22 +1630,22 @@
       </c>
       <c r="O5" s="25">
         <f t="shared" ref="O5:O17" si="1">(SUM(G5,I5,K5,M5))/3600</f>
-        <v>0.05</v>
+        <v>1.6666666666666666E-2</v>
       </c>
       <c r="P5" s="20">
         <f t="shared" ref="P5:P17" si="2">(B5*N5)+(D5*O5)</f>
-        <v>0.25</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="Q5" s="14">
         <f t="shared" ref="Q5:Q17" si="3">(C5*N5)+(E5*O5)</f>
-        <v>0.4</v>
-      </c>
-      <c r="R5" s="54" t="s">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="R5" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="S5" s="55"/>
-      <c r="T5" s="55"/>
-      <c r="U5" s="67"/>
+      <c r="S5" s="60"/>
+      <c r="T5" s="60"/>
+      <c r="U5" s="65"/>
       <c r="V5" s="33"/>
     </row>
     <row r="6" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1667,7 +1671,7 @@
         <v>10</v>
       </c>
       <c r="H6" s="42">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="I6" s="44">
         <v>0</v>
@@ -1686,7 +1690,7 @@
       </c>
       <c r="N6" s="24">
         <f t="shared" si="0"/>
-        <v>4.7222222222222221E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="O6" s="25">
         <f t="shared" si="1"/>
@@ -1700,12 +1704,12 @@
         <f t="shared" si="3"/>
         <v>1.3888888888888888</v>
       </c>
-      <c r="R6" s="54" t="s">
+      <c r="R6" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="S6" s="55"/>
-      <c r="T6" s="55"/>
-      <c r="U6" s="67"/>
+      <c r="S6" s="60"/>
+      <c r="T6" s="60"/>
+      <c r="U6" s="65"/>
       <c r="V6" s="33"/>
     </row>
     <row r="7" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1764,12 +1768,12 @@
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="R7" s="54" t="s">
+      <c r="R7" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="S7" s="55"/>
-      <c r="T7" s="55"/>
-      <c r="U7" s="55"/>
+      <c r="S7" s="60"/>
+      <c r="T7" s="60"/>
+      <c r="U7" s="60"/>
       <c r="V7" s="33"/>
     </row>
     <row r="8" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1828,12 +1832,12 @@
         <f t="shared" si="3"/>
         <v>2.4305555555555556E-2</v>
       </c>
-      <c r="R8" s="73" t="s">
+      <c r="R8" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="S8" s="74"/>
-      <c r="T8" s="74"/>
-      <c r="U8" s="74"/>
+      <c r="S8" s="62"/>
+      <c r="T8" s="62"/>
+      <c r="U8" s="62"/>
       <c r="V8" s="33"/>
     </row>
     <row r="9" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1892,17 +1896,17 @@
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="R9" s="75" t="s">
+      <c r="R9" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="S9" s="76"/>
-      <c r="T9" s="76"/>
-      <c r="U9" s="76"/>
+      <c r="S9" s="64"/>
+      <c r="T9" s="64"/>
+      <c r="U9" s="64"/>
       <c r="V9" s="33"/>
     </row>
     <row r="10" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="31" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -1926,7 +1930,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="44">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="J10" s="42">
         <v>0</v>
@@ -1946,26 +1950,26 @@
       </c>
       <c r="O10" s="25">
         <f t="shared" si="1"/>
-        <v>4.4444444444444446E-2</v>
+        <v>1.1111111111111112E-2</v>
       </c>
       <c r="P10" s="20">
         <f t="shared" si="2"/>
-        <v>1.3333333333333335</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="Q10" s="14">
         <f t="shared" si="3"/>
-        <v>1.7777777777777779</v>
-      </c>
-      <c r="R10" s="54" t="s">
+        <v>0.44444444444444448</v>
+      </c>
+      <c r="R10" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="S10" s="55"/>
-      <c r="T10" s="55"/>
-      <c r="U10" s="67"/>
+      <c r="S10" s="60"/>
+      <c r="T10" s="60"/>
+      <c r="U10" s="65"/>
     </row>
     <row r="11" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="6">
         <v>4</v>
@@ -1986,10 +1990,10 @@
         <v>0</v>
       </c>
       <c r="H11" s="42">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="I11" s="44">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J11" s="42">
         <v>30</v>
@@ -2005,26 +2009,26 @@
       </c>
       <c r="N11" s="24">
         <f t="shared" si="0"/>
-        <v>4.4444444444444446E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="O11" s="25">
         <f t="shared" si="1"/>
-        <v>5.5555555555555558E-3</v>
+        <v>2.7777777777777779E-3</v>
       </c>
       <c r="P11" s="20">
         <f t="shared" si="2"/>
-        <v>1.0666666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="Q11" s="14">
         <f t="shared" si="3"/>
-        <v>1.2222222222222223</v>
-      </c>
-      <c r="R11" s="54" t="s">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="R11" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="S11" s="55"/>
-      <c r="T11" s="55"/>
-      <c r="U11" s="67"/>
+      <c r="S11" s="60"/>
+      <c r="T11" s="60"/>
+      <c r="U11" s="65"/>
     </row>
     <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="32"/>
@@ -2036,27 +2040,27 @@
       <c r="G12" s="44"/>
       <c r="H12" s="42"/>
       <c r="I12" s="44">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J12" s="42">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K12" s="44">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="L12" s="42">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M12" s="44">
         <v>0</v>
       </c>
       <c r="N12" s="24">
         <f t="shared" si="0"/>
-        <v>5.5555555555555558E-3</v>
+        <v>0</v>
       </c>
       <c r="O12" s="25">
         <f t="shared" si="1"/>
-        <v>3.6111111111111108E-2</v>
+        <v>0</v>
       </c>
       <c r="P12" s="20">
         <f t="shared" si="2"/>
@@ -2066,12 +2070,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R12" s="54" t="s">
+      <c r="R12" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="S12" s="55"/>
-      <c r="T12" s="55"/>
-      <c r="U12" s="67"/>
+      <c r="S12" s="60"/>
+      <c r="T12" s="60"/>
+      <c r="U12" s="65"/>
     </row>
     <row r="13" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="32"/>
@@ -2103,12 +2107,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R13" s="54" t="s">
+      <c r="R13" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="S13" s="55"/>
-      <c r="T13" s="55"/>
-      <c r="U13" s="67"/>
+      <c r="S13" s="60"/>
+      <c r="T13" s="60"/>
+      <c r="U13" s="65"/>
     </row>
     <row r="14" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="32"/>
@@ -2140,12 +2144,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R14" s="54" t="s">
+      <c r="R14" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="S14" s="55"/>
-      <c r="T14" s="55"/>
-      <c r="U14" s="67"/>
+      <c r="S14" s="60"/>
+      <c r="T14" s="60"/>
+      <c r="U14" s="65"/>
       <c r="V14" s="33"/>
     </row>
     <row r="15" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2178,12 +2182,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R15" s="54" t="s">
+      <c r="R15" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="S15" s="55"/>
-      <c r="T15" s="55"/>
-      <c r="U15" s="67"/>
+      <c r="S15" s="60"/>
+      <c r="T15" s="60"/>
+      <c r="U15" s="65"/>
       <c r="V15" s="33"/>
     </row>
     <row r="16" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2216,12 +2220,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R16" s="54" t="s">
+      <c r="R16" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="S16" s="55"/>
-      <c r="T16" s="55"/>
-      <c r="U16" s="55"/>
+      <c r="S16" s="60"/>
+      <c r="T16" s="60"/>
+      <c r="U16" s="60"/>
       <c r="V16" s="33"/>
     </row>
     <row r="17" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2254,72 +2258,72 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R17" s="54" t="s">
+      <c r="R17" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="S17" s="55"/>
-      <c r="T17" s="55"/>
-      <c r="U17" s="55"/>
+      <c r="S17" s="60"/>
+      <c r="T17" s="60"/>
+      <c r="U17" s="60"/>
       <c r="V17" s="33"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A18" s="71" t="s">
+      <c r="A18" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="71"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="71"/>
-      <c r="K18" s="71"/>
-      <c r="L18" s="71"/>
-      <c r="M18" s="72"/>
-      <c r="N18" s="77" t="s">
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="58"/>
+      <c r="N18" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="O18" s="78"/>
-      <c r="P18" s="65">
+      <c r="O18" s="67"/>
+      <c r="P18" s="70">
         <f>SUM(P4:P17)</f>
-        <v>12.263194444444444</v>
-      </c>
-      <c r="Q18" s="65">
+        <v>10.61875</v>
+      </c>
+      <c r="Q18" s="70">
         <f>SUM(Q4:Q17)</f>
-        <v>20.882638888888888</v>
+        <v>18.807638888888885</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="N19" s="79"/>
-      <c r="O19" s="80"/>
-      <c r="P19" s="66"/>
-      <c r="Q19" s="66"/>
+      <c r="N19" s="68"/>
+      <c r="O19" s="69"/>
+      <c r="P19" s="71"/>
+      <c r="Q19" s="71"/>
     </row>
     <row r="20" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="N20" s="52" t="s">
+      <c r="N20" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="O20" s="53"/>
-      <c r="P20" s="52">
+      <c r="O20" s="73"/>
+      <c r="P20" s="72">
         <v>2400</v>
       </c>
-      <c r="Q20" s="62"/>
+      <c r="Q20" s="80"/>
       <c r="R20" s="9"/>
     </row>
     <row r="21" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="N21" s="52" t="s">
+      <c r="N21" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="O21" s="53"/>
+      <c r="O21" s="73"/>
       <c r="P21" s="35">
         <f>(P20/P18)</f>
-        <v>195.70757121014779</v>
+        <v>226.01530311948204</v>
       </c>
       <c r="Q21" s="36">
         <f>(P20/Q18)</f>
-        <v>114.92800372451865</v>
+        <v>127.6077244027619</v>
       </c>
       <c r="R21" s="9"/>
     </row>
@@ -2376,12 +2380,17 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="F1:M1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="R17:U17"/>
+    <mergeCell ref="R2:U3"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="R6:U6"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="R4:U4"/>
     <mergeCell ref="A18:M18"/>
     <mergeCell ref="R7:U7"/>
     <mergeCell ref="R8:U8"/>
@@ -2395,17 +2404,12 @@
     <mergeCell ref="R16:U16"/>
     <mergeCell ref="N18:O19"/>
     <mergeCell ref="P18:P19"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="R17:U17"/>
-    <mergeCell ref="R2:U3"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="Q18:Q19"/>
-    <mergeCell ref="R6:U6"/>
-    <mergeCell ref="R5:U5"/>
-    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="F1:M1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="73" orientation="landscape" r:id="rId1"/>

</xml_diff>